<commit_message>
update check_data for excel
</commit_message>
<xml_diff>
--- a/src/menu/admin/Menu.xlsx
+++ b/src/menu/admin/Menu.xlsx
@@ -325,14 +325,14 @@
   <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.88671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.9921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="49.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="77.71"/>
   </cols>

</xml_diff>

<commit_message>
Added missing type hints
</commit_message>
<xml_diff>
--- a/src/menu/admin/Menu.xlsx
+++ b/src/menu/admin/Menu.xlsx
@@ -324,11 +324,11 @@
   </sheetPr>
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:F18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.9921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.92"/>

</xml_diff>